<commit_message>
Excel now reads all tabs except custom equipment
</commit_message>
<xml_diff>
--- a/templates/excel_template.xlsx
+++ b/templates/excel_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neiman/Documents/Projects/Coding/nplcore/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neiman/Documents/Projects/Coding/nplcore/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7F9B44-6BE8-E44A-94BF-614C44577BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56860CB-9310-4640-88B2-BDB26C0B364D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" activeTab="1" xr2:uid="{88D35EFF-2385-9E4C-A9AE-1ECABB4945D7}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" activeTab="3" xr2:uid="{88D35EFF-2385-9E4C-A9AE-1ECABB4945D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Monday</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>Quarter End Date</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Holidays</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C731D31-1B7D-F741-9123-3E1742684EBB}" name="Table1" displayName="Table1" ref="A3:F14" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C731D31-1B7D-F741-9123-3E1742684EBB}" name="TechsTable" displayName="TechsTable" ref="A3:F14" totalsRowShown="0">
   <autoFilter ref="A3:F14" xr:uid="{2C731D31-1B7D-F741-9123-3E1742684EBB}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{DC8F43C6-7C72-E14B-9FBA-F1D9A84FB527}" name=" " dataDxfId="5"/>
@@ -449,22 +455,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4AB8D37-1A20-E94E-8ADE-8B6B0D6FC4CE}" name="Table2" displayName="Table2" ref="A3:F4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4AB8D37-1A20-E94E-8ADE-8B6B0D6FC4CE}" name="SectionsTable" displayName="SectionsTable" ref="A3:F4" totalsRowShown="0">
   <autoFilter ref="A3:F4" xr:uid="{C4AB8D37-1A20-E94E-8ADE-8B6B0D6FC4CE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{DF1E1428-B694-6D48-9D7C-0006DD48B384}" name="Course Number"/>
     <tableColumn id="2" xr3:uid="{ADE78419-7756-3E4E-98C9-797C225C9A8E}" name="Section"/>
     <tableColumn id="3" xr3:uid="{3458D087-DB74-4347-8CD8-34D88BE9FA63}" name="Instructor"/>
     <tableColumn id="4" xr3:uid="{E4E11555-0E27-5A43-B587-02115FC7545E}" name="Room"/>
+    <tableColumn id="6" xr3:uid="{3910A0E2-94C8-6A4D-877D-B5A46C4C4266}" name="Day of Week"/>
     <tableColumn id="5" xr3:uid="{B4383917-8937-2B4E-B158-413C61D1D589}" name="Start Time"/>
-    <tableColumn id="6" xr3:uid="{3910A0E2-94C8-6A4D-877D-B5A46C4C4266}" name="Day of Week"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{80429304-9240-664F-8471-B6C297D3E411}" name="Table7" displayName="Table7" ref="H3:I4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{80429304-9240-664F-8471-B6C297D3E411}" name="DatesTable" displayName="DatesTable" ref="H3:I4" totalsRowShown="0">
   <autoFilter ref="H3:I4" xr:uid="{80429304-9240-664F-8471-B6C297D3E411}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{66DB4DBA-700D-3A49-8FA0-9A79581DBD98}" name="Quarter Start Date"/>
@@ -475,7 +481,17 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A4ABDCEB-6C5C-8E44-900C-3E059605AD75}" name="Table4" displayName="Table4" ref="A3:C6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03462755-0876-8247-89A8-52072B85C9C1}" name="Table3" displayName="Table3" ref="K3:K4" totalsRowShown="0">
+  <autoFilter ref="K3:K4" xr:uid="{03462755-0876-8247-89A8-52072B85C9C1}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{BC6C4B4F-C96C-CF49-9C4B-68FB349DF5E5}" name="Holidays"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A4ABDCEB-6C5C-8E44-900C-3E059605AD75}" name="InventoryTable" displayName="InventoryTable" ref="A3:C6" totalsRowShown="0">
   <autoFilter ref="A3:C6" xr:uid="{A4ABDCEB-6C5C-8E44-900C-3E059605AD75}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{12A6EAEF-1AEF-1E4C-A321-EF796BA89955}" name="Desc"/>
@@ -486,12 +502,14 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2972FD81-A2A4-5E46-8FFB-23592027551D}" name="Table6" displayName="Table6" ref="A3:R4" totalsRowShown="0">
-  <autoFilter ref="A3:R4" xr:uid="{2972FD81-A2A4-5E46-8FFB-23592027551D}"/>
-  <tableColumns count="18">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2972FD81-A2A4-5E46-8FFB-23592027551D}" name="DefaultReqsTable" displayName="DefaultReqsTable" ref="A3:T4" totalsRowShown="0">
+  <autoFilter ref="A3:T4" xr:uid="{2972FD81-A2A4-5E46-8FFB-23592027551D}"/>
+  <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{815AE0A1-9197-2242-870D-3F564CB963DF}" name="Class"/>
     <tableColumn id="2" xr3:uid="{A6CC93D6-98CD-164C-9E50-7DDBCAAE99E7}" name="Week"/>
+    <tableColumn id="19" xr3:uid="{147EA289-ABA0-6543-9040-A5F26597C3CE}" name="Note"/>
+    <tableColumn id="20" xr3:uid="{5F44EF4B-AD18-3B45-9BCE-46A42F256325}" name="Shortcode"/>
     <tableColumn id="3" xr3:uid="{F5C8C0DC-85F1-1840-A2CE-13FAD10AC702}" name="Equipment"/>
     <tableColumn id="4" xr3:uid="{7C5ACFC7-BAC6-2D4B-ABE0-E96ECBB3ABF7}" name="Qty"/>
     <tableColumn id="5" xr3:uid="{753E63A1-1FF4-EE46-8C24-88AAD47E1E0D}" name="Equipment2"/>
@@ -513,8 +531,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}" name="Table5" displayName="Table5" ref="A3:L4" totalsRowShown="0">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}" name="CustomModsTable" displayName="CustomModsTable" ref="A3:L4" totalsRowShown="0">
   <autoFilter ref="A3:L4" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{438C46B6-0993-5F49-8874-8162B699718F}" name="Section"/>
@@ -833,7 +851,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6698079-A529-9243-A264-09F05A293C2C}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -991,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8B4231-362B-584F-8425-770C395E0704}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1002,13 +1022,13 @@
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -1017,7 +1037,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1031,10 +1051,10 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>57</v>
       </c>
       <c r="H3" t="s">
         <v>58</v>
@@ -1042,12 +1062,16 @@
       <c r="I3" t="s">
         <v>59</v>
       </c>
+      <c r="K3" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1057,7 +1081,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1111,6 +1135,9 @@
       <c r="A6" t="s">
         <v>25</v>
       </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
       <c r="C6" t="s">
         <v>26</v>
       </c>
@@ -1125,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CC2DBF-3E41-6646-A163-F2349C1EDF4A}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1170,7 @@
     <col min="17" max="17" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1151,7 +1178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1159,51 +1186,57 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>43</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>44</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>45</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>46</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>47</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>48</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>49</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>50</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>51</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>52</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>54</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1220,7 +1253,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Now takes lab groups
</commit_message>
<xml_diff>
--- a/templates/excel_template.xlsx
+++ b/templates/excel_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neiman/Documents/Projects/Coding/nplcore/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56860CB-9310-4640-88B2-BDB26C0B364D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4752933-B147-8A4D-9EAC-50B8B64B286F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" activeTab="3" xr2:uid="{88D35EFF-2385-9E4C-A9AE-1ECABB4945D7}"/>
+    <workbookView xWindow="780" yWindow="1860" windowWidth="28040" windowHeight="17260" activeTab="1" xr2:uid="{88D35EFF-2385-9E4C-A9AE-1ECABB4945D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
   <si>
     <t>Monday</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Lab Tech Schedule</t>
   </si>
   <si>
-    <t>Which equipment required for each default section</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
@@ -136,36 +133,6 @@
     <t>Special order for lab instructor equipment</t>
   </si>
   <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t>Week 6</t>
-  </si>
-  <si>
-    <t>Week 7</t>
-  </si>
-  <si>
-    <t>Week 8</t>
-  </si>
-  <si>
-    <t>Week 9</t>
-  </si>
-  <si>
-    <t>Week 10</t>
-  </si>
-  <si>
     <t>Equipment2</t>
   </si>
   <si>
@@ -223,7 +190,52 @@
     <t>Note</t>
   </si>
   <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Natalie</t>
+  </si>
+  <si>
+    <t>Xaviera</t>
+  </si>
+  <si>
+    <t>Shalini</t>
+  </si>
+  <si>
+    <t>Edgar</t>
+  </si>
+  <si>
+    <t>Weston</t>
+  </si>
+  <si>
+    <t>Indigo</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Poshtan</t>
+  </si>
+  <si>
+    <t>McDonald</t>
+  </si>
+  <si>
     <t>Holidays</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Num. Groups</t>
+  </si>
+  <si>
+    <t>Which equipment required for each default section- PER GROUP REQUIREMEBNTS, not total</t>
   </si>
 </sst>
 </file>
@@ -296,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -308,6 +320,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,23 +470,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4AB8D37-1A20-E94E-8ADE-8B6B0D6FC4CE}" name="SectionsTable" displayName="SectionsTable" ref="A3:F4" totalsRowShown="0">
-  <autoFilter ref="A3:F4" xr:uid="{C4AB8D37-1A20-E94E-8ADE-8B6B0D6FC4CE}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4AB8D37-1A20-E94E-8ADE-8B6B0D6FC4CE}" name="SectionsTable" displayName="SectionsTable" ref="A3:G5" totalsRowShown="0">
+  <autoFilter ref="A3:G5" xr:uid="{C4AB8D37-1A20-E94E-8ADE-8B6B0D6FC4CE}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DF1E1428-B694-6D48-9D7C-0006DD48B384}" name="Course Number"/>
     <tableColumn id="2" xr3:uid="{ADE78419-7756-3E4E-98C9-797C225C9A8E}" name="Section"/>
     <tableColumn id="3" xr3:uid="{3458D087-DB74-4347-8CD8-34D88BE9FA63}" name="Instructor"/>
     <tableColumn id="4" xr3:uid="{E4E11555-0E27-5A43-B587-02115FC7545E}" name="Room"/>
     <tableColumn id="6" xr3:uid="{3910A0E2-94C8-6A4D-877D-B5A46C4C4266}" name="Day of Week"/>
     <tableColumn id="5" xr3:uid="{B4383917-8937-2B4E-B158-413C61D1D589}" name="Start Time"/>
+    <tableColumn id="7" xr3:uid="{6A02BF4C-6A17-7C4E-B184-CB9B75E5D965}" name="Num. Groups"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{80429304-9240-664F-8471-B6C297D3E411}" name="DatesTable" displayName="DatesTable" ref="H3:I4" totalsRowShown="0">
-  <autoFilter ref="H3:I4" xr:uid="{80429304-9240-664F-8471-B6C297D3E411}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{80429304-9240-664F-8471-B6C297D3E411}" name="DatesTable" displayName="DatesTable" ref="I3:J4" totalsRowShown="0">
+  <autoFilter ref="I3:J4" xr:uid="{80429304-9240-664F-8471-B6C297D3E411}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{66DB4DBA-700D-3A49-8FA0-9A79581DBD98}" name="Quarter Start Date"/>
     <tableColumn id="2" xr3:uid="{79BD2CF2-D015-8E4D-9923-8E1330F87625}" name="Quarter End Date"/>
@@ -481,10 +497,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03462755-0876-8247-89A8-52072B85C9C1}" name="Table3" displayName="Table3" ref="K3:K4" totalsRowShown="0">
-  <autoFilter ref="K3:K4" xr:uid="{03462755-0876-8247-89A8-52072B85C9C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6C536572-B9D0-EB46-85F1-1A565842F3A7}" name="Table3" displayName="Table3" ref="L3:L7" totalsRowShown="0">
+  <autoFilter ref="L3:L7" xr:uid="{6C536572-B9D0-EB46-85F1-1A565842F3A7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{BC6C4B4F-C96C-CF49-9C4B-68FB349DF5E5}" name="Holidays"/>
+    <tableColumn id="1" xr3:uid="{8C9431BB-8888-8C45-84C8-48856E213DBE}" name="Holidays"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -509,7 +525,7 @@
     <tableColumn id="1" xr3:uid="{815AE0A1-9197-2242-870D-3F564CB963DF}" name="Class"/>
     <tableColumn id="2" xr3:uid="{A6CC93D6-98CD-164C-9E50-7DDBCAAE99E7}" name="Week"/>
     <tableColumn id="19" xr3:uid="{147EA289-ABA0-6543-9040-A5F26597C3CE}" name="Note"/>
-    <tableColumn id="20" xr3:uid="{5F44EF4B-AD18-3B45-9BCE-46A42F256325}" name="Shortcode"/>
+    <tableColumn id="20" xr3:uid="{73F2CEEB-CDC1-A144-AEAC-A0029BAE876F}" name="Shortcode"/>
     <tableColumn id="3" xr3:uid="{F5C8C0DC-85F1-1840-A2CE-13FAD10AC702}" name="Equipment"/>
     <tableColumn id="4" xr3:uid="{7C5ACFC7-BAC6-2D4B-ABE0-E96ECBB3ABF7}" name="Qty"/>
     <tableColumn id="5" xr3:uid="{753E63A1-1FF4-EE46-8C24-88AAD47E1E0D}" name="Equipment2"/>
@@ -532,21 +548,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}" name="CustomModsTable" displayName="CustomModsTable" ref="A3:L4" totalsRowShown="0">
-  <autoFilter ref="A3:L4" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}" name="CustomModsTable" displayName="CustomModsTable" ref="A3:E4" totalsRowShown="0">
+  <autoFilter ref="A3:E4" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{438C46B6-0993-5F49-8874-8162B699718F}" name="Section"/>
     <tableColumn id="2" xr3:uid="{9A88EC7A-E958-EB4B-B54B-09FB4E7C723B}" name="Instructor"/>
-    <tableColumn id="3" xr3:uid="{BD1B8B4E-AD26-184E-9A9A-38494EC2D7C1}" name="Week 1"/>
-    <tableColumn id="4" xr3:uid="{D12C408E-B189-9141-81E3-AEF9D0C7D7B7}" name="Week 2"/>
-    <tableColumn id="5" xr3:uid="{928EF546-A412-D442-A344-E167ECF383FC}" name="Week 3"/>
-    <tableColumn id="6" xr3:uid="{F79D9492-14AE-634A-896F-05C01F256C33}" name="Week 4"/>
-    <tableColumn id="7" xr3:uid="{117AA407-15CF-CA44-906A-57C8A08AAC27}" name="Week 5"/>
-    <tableColumn id="8" xr3:uid="{2A4E07D2-FA67-8843-8758-AF40CFDE1714}" name="Week 6"/>
-    <tableColumn id="9" xr3:uid="{093BC436-D255-9940-94FF-CA10241445A5}" name="Week 7"/>
-    <tableColumn id="10" xr3:uid="{F2A56A94-A7EB-9D40-A5E7-97805E757601}" name="Week 8"/>
-    <tableColumn id="11" xr3:uid="{7DCA2D72-715B-F84C-8800-B3581A3F332F}" name="Week 9"/>
-    <tableColumn id="12" xr3:uid="{750D4C53-9EC8-064E-B192-CCCBAA4D5716}" name="Week 10"/>
+    <tableColumn id="3" xr3:uid="{BD1B8B4E-AD26-184E-9A9A-38494EC2D7C1}" name="Week"/>
+    <tableColumn id="4" xr3:uid="{D12C408E-B189-9141-81E3-AEF9D0C7D7B7}" name="Time"/>
+    <tableColumn id="5" xr3:uid="{928EF546-A412-D442-A344-E167ECF383FC}" name="Equipment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -852,7 +861,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -895,110 +904,216 @@
       <c r="A4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.375</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0.5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0.625</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0.75</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="F14" s="3"/>
     </row>
   </sheetData>
@@ -1011,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8B4231-362B-584F-8425-770C395E0704}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1024,20 +1139,21 @@
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1051,19 +1167,84 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
-        <v>58</v>
+      <c r="G3" t="s">
+        <v>64</v>
       </c>
       <c r="I3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>295</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>102</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I4" s="8">
+        <v>45176</v>
+      </c>
+      <c r="J4" s="8">
+        <v>45268</v>
+      </c>
+      <c r="L4" s="9">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>251</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>61</v>
+      </c>
+      <c r="D5">
+        <v>113</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="9">
+        <v>45263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L6" s="9">
+        <v>45265</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L7" s="9">
+        <v>45259</v>
       </c>
     </row>
   </sheetData>
@@ -1092,54 +1273,54 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1154,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CC2DBF-3E41-6646-A163-F2349C1EDF4A}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1172,72 +1353,72 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
       <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" t="s">
         <v>42</v>
       </c>
-      <c r="H3" t="s">
+      <c r="S3" t="s">
         <v>43</v>
       </c>
-      <c r="I3" t="s">
+      <c r="T3" t="s">
         <v>44</v>
-      </c>
-      <c r="J3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R3" t="s">
-        <v>53</v>
-      </c>
-      <c r="S3" t="s">
-        <v>54</v>
-      </c>
-      <c r="T3" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1250,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F056D647-2C2A-4240-8D5C-FF0F5D3E080D}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1261,15 +1442,15 @@
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1277,34 +1458,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>